<commit_message>
Handling variable metadata for data requests
</commit_message>
<xml_diff>
--- a/tests/example_inputs/variables.xlsx
+++ b/tests/example_inputs/variables.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Born In Bradford - Confidential\Opal\epivaultr\tests\example_inputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D65EF01-238E-4106-BC65-3D445D6304B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="5460"/>
+    <workbookView xWindow="-4110" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>variable</t>
   </si>
@@ -28,18 +34,6 @@
     <t>BiBBS_Baseline.pregnancy_survey.adm_qpresent</t>
   </si>
   <si>
-    <t>BiBBS_Baseline.pregnancy_survey.mes1_weighttaken</t>
-  </si>
-  <si>
-    <t>BiBBS_Baseline.pregnancy_survey.mes1_qweight</t>
-  </si>
-  <si>
-    <t>BiBBS_Baseline.pregnancy_survey.mes1_bmicalc</t>
-  </si>
-  <si>
-    <t>BiBBS_Baseline.pregnancy_survey.mes1_triceptaken</t>
-  </si>
-  <si>
     <t>BiBBS_Baseline.pregnancy_survey.res_4plsoacode</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
     <t>BiBBS_Baseline.pregnancy_survey.lng_3child_other</t>
   </si>
   <si>
-    <t>BiBBS_Baseline.pregnancy_survey.fin_2cutmeals</t>
-  </si>
-  <si>
     <t>BiBBS_Baseline.pregnancy_survey.soc_1_present</t>
   </si>
   <si>
@@ -67,22 +58,25 @@
     <t>BiBBS_CohortInfo.pregnancy.BiBBSPregnancyID</t>
   </si>
   <si>
-    <t>BiBBS_CohortInfo.pregnancy.medway_booking_y</t>
-  </si>
-  <si>
-    <t>BiBBS_CohortInfo.pregnancy.medway_booking_m</t>
-  </si>
-  <si>
     <t>BiBBS_CohortInfo.pregnancy.recrutiment_year</t>
   </si>
   <si>
     <t>BiBBS_CohortInfo.pregnancy.recrutiment_month</t>
+  </si>
+  <si>
+    <t>BiBBS_Baseline.pregnancy_survey.mes1_*</t>
+  </si>
+  <si>
+    <t>BiBBS_Baseline.pregnancy_survey.fin_?cutmeals</t>
+  </si>
+  <si>
+    <t>BiBBS_CohortInfo.pregnancy.medway_booking_?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,6 +608,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -661,7 +658,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,9 +691,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -729,6 +743,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -904,11 +935,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,87 +966,67 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basic handling of variable visibility level
</commit_message>
<xml_diff>
--- a/tests/example_inputs/variables.xlsx
+++ b/tests/example_inputs/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Born In Bradford - Confidential\Opal\epivaultr\tests\example_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D65EF01-238E-4106-BC65-3D445D6304B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01CA178-9AE1-44BC-9DAE-E4C643B164D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4110" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>variable</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>BiBBS_CohortInfo.pregnancy.medway_booking_?</t>
+  </si>
+  <si>
+    <t>BiBBS_CohortInfo.pregnancy.recruitment_date</t>
   </si>
 </sst>
 </file>
@@ -936,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,6 +1032,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SQL object type fix
</commit_message>
<xml_diff>
--- a/tests/example_inputs/variables.xlsx
+++ b/tests/example_inputs/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Born In Bradford - Confidential\Opal\epivaultr\tests\example_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01CA178-9AE1-44BC-9DAE-E4C643B164D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E586D0-875A-403C-94B9-51CE4A6AA230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4110" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>variable</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>BiBBS_CohortInfo.pregnancy.recruitment_date</t>
+  </si>
+  <si>
+    <t>BiB_Metabolomics.metms_pairm_s.metmss42370</t>
+  </si>
+  <si>
+    <t>BiB_Metabolomics.metms_pairm_s.metmss485</t>
+  </si>
+  <si>
+    <t>BiB_Metabolomics.metms_pairm_s.*</t>
   </si>
 </sst>
 </file>
@@ -939,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,6 +1046,21 @@
         <v>17</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>